<commit_message>
changed background pictures and updated read/write for csv
</commit_message>
<xml_diff>
--- a/EE104_Lab2/Registration_UserName_Password.xlsx
+++ b/EE104_Lab2/Registration_UserName_Password.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD6"/>
@@ -465,6 +465,18 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>pranavk</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Pranav10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>